<commit_message>
fix(.), feat(.): project finishedd, features added and repaired bugs
</commit_message>
<xml_diff>
--- a/TodoListApp/results/task_report_excel.xlsx
+++ b/TodoListApp/results/task_report_excel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Tasks List from Todo</t>
   </si>
@@ -32,15 +32,39 @@
     <t>Due Date</t>
   </si>
   <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Tarea Cultura</t>
+  </si>
+  <si>
+    <t>Hacer el reporte de cultura</t>
+  </si>
+  <si>
+    <t>2023-10-31</t>
+  </si>
+  <si>
+    <t>Personal</t>
+  </si>
+  <si>
+    <t>Tarea Simulación</t>
+  </si>
+  <si>
+    <t>Hacer las distribuciones</t>
+  </si>
+  <si>
+    <t>2023-11-14</t>
+  </si>
+  <si>
+    <t>Simulación, ITC</t>
+  </si>
+  <si>
     <t>Tarea Taller</t>
   </si>
   <si>
     <t>Hacer el Laboratorio de TBD</t>
   </si>
   <si>
-    <t>2023-10-31</t>
-  </si>
-  <si>
     <t>Tarea Topicos</t>
   </si>
   <si>
@@ -50,10 +74,19 @@
     <t>2023-11-17</t>
   </si>
   <si>
-    <t>Tarea Cultura</t>
-  </si>
-  <si>
-    <t>Hacer el reporte de cultura</t>
+    <t>Personal,ITC</t>
+  </si>
+  <si>
+    <t>Tarea SO</t>
+  </si>
+  <si>
+    <t>Montar maquina virtual</t>
+  </si>
+  <si>
+    <t>2023-11-13</t>
+  </si>
+  <si>
+    <t>ITC,Sistemas operativos</t>
   </si>
 </sst>
 </file>
@@ -107,17 +140,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="6.75" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.18359375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="13.59765625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="23.31640625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="5.4921875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="9.421875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="18.54296875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -141,56 +175,108 @@
       <c r="E2" t="s" s="0">
         <v>5</v>
       </c>
+      <c r="F2" t="s" s="0">
+        <v>6</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n" s="0">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="b" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n" s="0">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D4" t="b" s="0">
         <v>0</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n" s="0">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D5" t="b" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D6" t="b" s="0">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D7" t="b" s="0">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>